<commit_message>
Ecoregions tab UX overhaul: map/list sync, bioregion metadata, click navigation
- Map now shows child features matching the list (not parent geometry)
- Added geometry endpoints: subrealms/geom, bioregions/geom, ecoregions/geom
- Distinct colors, hover highlighting, bidirectional map-list sync
- Bioregion titles from bioregion_meta table, OneEarth external links
- Click map features to drill down (same as clicking list item)
- Fixed WHG API input visibility on initial page load

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/output/missing_for_review_with_extracts.xlsx
+++ b/output/missing_for_review_with_extracts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlg/Documents/Repos/_edop/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80F3A6A-4101-804C-825C-5E371887689B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53C1EEB-1DA6-F546-A9E9-2FE135B64369}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="1180" windowWidth="27640" windowHeight="16920" xr2:uid="{13F9CCF1-9DC8-474E-93ED-6520C2A4DF72}"/>
   </bookViews>
@@ -1570,8 +1570,8 @@
   <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G71" sqref="G71"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1580,9 +1580,9 @@
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="80.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="80.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="50.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="80.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -1606,13 +1606,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>5</v>
@@ -1644,13 +1644,13 @@
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="4">
         <v>79.069767441860407</v>
@@ -1679,13 +1679,13 @@
         <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="H3" s="4">
         <v>100</v>
@@ -1711,13 +1711,13 @@
         <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="H4" s="4">
         <v>66.6666666666666</v>
@@ -1746,13 +1746,13 @@
         <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="H5" s="4">
         <v>66.6666666666666</v>
@@ -1781,13 +1781,13 @@
         <v>40</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="H6" s="4">
         <v>69.767441860465098</v>
@@ -1816,13 +1816,13 @@
         <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="H7" s="4">
         <v>29.629629629629601</v>
@@ -1851,13 +1851,13 @@
         <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="H8" s="4">
         <v>76.190476190476105</v>
@@ -1886,13 +1886,13 @@
         <v>55</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G9" s="1" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="H9" s="4">
         <v>75</v>
@@ -1921,13 +1921,13 @@
         <v>60</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="H10" s="4">
         <v>100</v>
@@ -1956,13 +1956,13 @@
         <v>65</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="H11" s="4">
         <v>66.6666666666666</v>
@@ -1991,13 +1991,13 @@
         <v>71</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="H12" s="4">
         <v>65.384615384615302</v>
@@ -2026,13 +2026,13 @@
         <v>76</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="H13" s="4">
         <v>100</v>
@@ -2058,13 +2058,13 @@
         <v>81</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="H14" s="4">
         <v>63.636363636363598</v>
@@ -2093,13 +2093,13 @@
         <v>86</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="H15" s="4">
         <v>50.909090909090899</v>
@@ -2128,13 +2128,13 @@
         <v>91</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="H16" s="4">
         <v>28.571428571428498</v>
@@ -2163,13 +2163,13 @@
         <v>96</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="H17" s="4">
         <v>62.5</v>
@@ -2198,13 +2198,13 @@
         <v>101</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="H18" s="4">
         <v>84.931506849314999</v>
@@ -2233,13 +2233,13 @@
         <v>107</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="H19" s="4">
         <v>79.069767441860407</v>
@@ -2268,13 +2268,13 @@
         <v>112</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="H20" s="4">
         <v>78.260869565217305</v>
@@ -2303,13 +2303,13 @@
         <v>118</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="H21" s="4">
         <v>61.1111111111111</v>
@@ -2338,13 +2338,13 @@
         <v>123</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>124</v>
+        <v>12</v>
       </c>
       <c r="H22" s="4">
         <v>73.3333333333333</v>
@@ -2373,13 +2373,13 @@
         <v>133</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>134</v>
+        <v>12</v>
       </c>
       <c r="H23" s="4">
         <v>58.3333333333333</v>
@@ -2408,13 +2408,13 @@
         <v>138</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G24" s="1" t="s">
-        <v>139</v>
+        <v>12</v>
       </c>
       <c r="H24" s="4">
         <v>63.157894736842103</v>
@@ -2443,13 +2443,13 @@
         <v>143</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="H25" s="4">
         <v>73.846153846153797</v>
@@ -2478,13 +2478,13 @@
         <v>149</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G26" s="1" t="s">
-        <v>150</v>
+        <v>12</v>
       </c>
       <c r="H26" s="4">
         <v>76.470588235294102</v>
@@ -2513,13 +2513,13 @@
         <v>154</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>155</v>
+        <v>12</v>
       </c>
       <c r="H27" s="4">
         <v>32</v>
@@ -2548,13 +2548,13 @@
         <v>159</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>160</v>
+        <v>12</v>
       </c>
       <c r="H28" s="4">
         <v>69.565217391304301</v>
@@ -2583,13 +2583,13 @@
         <v>164</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F29" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>165</v>
       </c>
       <c r="H29" s="4">
         <v>100</v>
@@ -2615,13 +2615,13 @@
         <v>169</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F30" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G30" s="1" t="s">
-        <v>170</v>
+        <v>12</v>
       </c>
       <c r="H30" s="4">
         <v>72.727272727272705</v>
@@ -2650,13 +2650,13 @@
         <v>174</v>
       </c>
       <c r="E31" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G31" s="1" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="H31" s="4">
         <v>49.056603773584897</v>
@@ -2685,13 +2685,13 @@
         <v>179</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="H32" s="4">
         <v>76.470588235294102</v>
@@ -2720,13 +2720,13 @@
         <v>185</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G33" s="1" t="s">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="H33" s="4">
         <v>71.428571428571402</v>
@@ -2755,13 +2755,13 @@
         <v>190</v>
       </c>
       <c r="E34" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G34" s="1" t="s">
-        <v>191</v>
+        <v>12</v>
       </c>
       <c r="H34" s="4">
         <v>77.7777777777777</v>
@@ -2790,13 +2790,13 @@
         <v>195</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G35" s="1" t="s">
-        <v>196</v>
+        <v>12</v>
       </c>
       <c r="H35" s="4">
         <v>70.588235294117595</v>
@@ -2825,13 +2825,13 @@
         <v>200</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="H36" s="4">
         <v>63.492063492063401</v>
@@ -2860,13 +2860,13 @@
         <v>206</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="G37" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="H37" s="4">
         <v>71.052631578947299</v>
@@ -2895,13 +2895,13 @@
         <v>212</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G38" s="1" t="s">
-        <v>213</v>
+        <v>12</v>
       </c>
       <c r="H38" s="4">
         <v>40</v>
@@ -2930,13 +2930,13 @@
         <v>217</v>
       </c>
       <c r="E39" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G39" s="1" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="H39" s="4">
         <v>46.428571428571402</v>
@@ -2965,13 +2965,13 @@
         <v>222</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F40" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="H40" s="4">
         <v>100</v>
@@ -2997,13 +2997,13 @@
         <v>224</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="F41" s="1" t="s">
+      <c r="G41" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>377</v>
       </c>
       <c r="H41" s="4">
         <v>60</v>
@@ -3032,13 +3032,13 @@
         <v>228</v>
       </c>
       <c r="E42" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F42" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="F42" s="1" t="s">
+      <c r="G42" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="H42" s="4">
         <v>69.387755102040799</v>
@@ -3067,13 +3067,13 @@
         <v>233</v>
       </c>
       <c r="E43" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F43" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F43" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G43" s="1" t="s">
-        <v>234</v>
+        <v>12</v>
       </c>
       <c r="H43" s="4">
         <v>81.967213114754102</v>
@@ -3102,13 +3102,13 @@
         <v>243</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F44" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G44" s="1" t="s">
-        <v>244</v>
+        <v>12</v>
       </c>
       <c r="H44" s="4">
         <v>75</v>
@@ -3137,13 +3137,13 @@
         <v>248</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="H45" s="4">
         <v>74.285714285714207</v>
@@ -3172,13 +3172,13 @@
         <v>253</v>
       </c>
       <c r="E46" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G46" s="1" t="s">
-        <v>254</v>
+        <v>12</v>
       </c>
       <c r="H46" s="4">
         <v>76.470588235294102</v>
@@ -3207,13 +3207,13 @@
         <v>258</v>
       </c>
       <c r="E47" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G47" s="1" t="s">
-        <v>259</v>
+        <v>12</v>
       </c>
       <c r="H47" s="4">
         <v>76.470588235294102</v>
@@ -3242,13 +3242,13 @@
         <v>263</v>
       </c>
       <c r="E48" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G48" s="1" t="s">
-        <v>264</v>
+        <v>12</v>
       </c>
       <c r="H48" s="4">
         <v>60</v>
@@ -3277,13 +3277,13 @@
         <v>272</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="H49" s="4">
         <v>71.052631578947299</v>
@@ -3312,13 +3312,13 @@
         <v>277</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G50" s="1" t="s">
-        <v>278</v>
+        <v>12</v>
       </c>
       <c r="H50" s="4">
         <v>100</v>
@@ -3347,13 +3347,13 @@
         <v>282</v>
       </c>
       <c r="E51" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G51" s="1" t="s">
-        <v>283</v>
+        <v>12</v>
       </c>
       <c r="H51" s="4">
         <v>35.714285714285701</v>
@@ -3382,13 +3382,13 @@
         <v>287</v>
       </c>
       <c r="E52" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>288</v>
       </c>
       <c r="H52" s="4">
         <v>79.518072289156606</v>
@@ -3417,13 +3417,13 @@
         <v>293</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="F53" s="1" t="s">
+      <c r="G53" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>375</v>
       </c>
       <c r="H53" s="4">
         <v>63.157894736842103</v>
@@ -3452,13 +3452,13 @@
         <v>296</v>
       </c>
       <c r="E54" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="F54" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>297</v>
       </c>
       <c r="H54" s="4">
         <v>75</v>
@@ -3487,13 +3487,13 @@
         <v>302</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>303</v>
       </c>
       <c r="H55" s="4">
         <v>89.156626506024097</v>
@@ -3519,13 +3519,13 @@
         <v>307</v>
       </c>
       <c r="E56" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="F56" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G56" s="1" t="s">
-        <v>308</v>
+        <v>12</v>
       </c>
       <c r="H56" s="4">
         <v>63.157894736842103</v>
@@ -3554,13 +3554,13 @@
         <v>312</v>
       </c>
       <c r="E57" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F57" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="F57" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G57" s="1" t="s">
-        <v>313</v>
+        <v>12</v>
       </c>
       <c r="H57" s="4">
         <v>58.9743589743589</v>
@@ -3589,13 +3589,13 @@
         <v>317</v>
       </c>
       <c r="E58" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G58" s="1" t="s">
-        <v>318</v>
+        <v>12</v>
       </c>
       <c r="H58" s="4">
         <v>52.747252747252702</v>
@@ -3624,13 +3624,13 @@
         <v>322</v>
       </c>
       <c r="E59" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="F59" s="1" t="s">
+      <c r="G59" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>318</v>
       </c>
       <c r="H59" s="4">
         <v>65.789473684210506</v>
@@ -3659,13 +3659,13 @@
         <v>325</v>
       </c>
       <c r="E60" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G60" s="1" t="s">
-        <v>326</v>
+        <v>12</v>
       </c>
       <c r="H60" s="4">
         <v>25</v>
@@ -3694,13 +3694,13 @@
         <v>330</v>
       </c>
       <c r="E61" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G61" s="1" t="s">
-        <v>331</v>
+        <v>12</v>
       </c>
       <c r="H61" s="4">
         <v>94.117647058823493</v>
@@ -3729,13 +3729,13 @@
         <v>335</v>
       </c>
       <c r="E62" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G62" s="1" t="s">
-        <v>336</v>
+        <v>12</v>
       </c>
       <c r="H62" s="4">
         <v>35.714285714285701</v>
@@ -3764,13 +3764,13 @@
         <v>340</v>
       </c>
       <c r="E63" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G63" s="1" t="s">
-        <v>341</v>
+        <v>12</v>
       </c>
       <c r="H63" s="4">
         <v>72.2222222222222</v>
@@ -3799,13 +3799,13 @@
         <v>346</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G64" s="1" t="s">
-        <v>347</v>
+        <v>12</v>
       </c>
       <c r="H64" s="4">
         <v>53.731343283582</v>
@@ -3834,13 +3834,13 @@
         <v>351</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G65" s="1" t="s">
-        <v>352</v>
+        <v>12</v>
       </c>
       <c r="H65" s="4">
         <v>64</v>
@@ -3869,13 +3869,13 @@
         <v>356</v>
       </c>
       <c r="E66" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F66" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G66" s="1" t="s">
-        <v>357</v>
+        <v>12</v>
       </c>
       <c r="H66" s="4">
         <v>68.421052631578902</v>
@@ -3904,13 +3904,13 @@
         <v>361</v>
       </c>
       <c r="E67" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="F67" s="1" t="s">
+      <c r="G67" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>362</v>
       </c>
       <c r="H67" s="4">
         <v>62.068965517241303</v>
@@ -3939,13 +3939,13 @@
         <v>345</v>
       </c>
       <c r="E68" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F68" s="1" t="s">
+      <c r="G68" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="H68" s="4">
         <v>100</v>
@@ -3971,13 +3971,13 @@
         <v>238</v>
       </c>
       <c r="E69" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="F69" s="1" t="s">
+      <c r="G69" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="H69" s="4">
         <v>100</v>
@@ -4003,13 +4003,13 @@
         <v>268</v>
       </c>
       <c r="E70" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="F70" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="H70" s="4">
         <v>67.647058823529406</v>
@@ -4038,13 +4038,13 @@
         <v>17</v>
       </c>
       <c r="E71" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F71" s="1" t="s">
+      <c r="G71" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="H71" s="4">
         <v>68.75</v>
@@ -4070,13 +4070,13 @@
         <v>128</v>
       </c>
       <c r="E72" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F72" s="1" t="s">
+      <c r="G72" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="H72" s="4">
         <v>66.6666666666666</v>

</xml_diff>